<commit_message>
Add detail analysis code for wang and marsden
</commit_message>
<xml_diff>
--- a/remote-results/results/cohen/cohen-results.xlsx
+++ b/remote-results/results/cohen/cohen-results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EEB379F-D9F3-45AD-AC59-8E788EB972DC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D734C1DE-AF5E-49E8-933B-09162EA093CC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="7008" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6433,7 +6433,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9097,7 +9097,7 @@
         <v>94.252197265625</v>
       </c>
       <c r="F98">
-        <f t="shared" ref="F98:F129" si="9">E98*E98</f>
+        <f t="shared" ref="F98:F101" si="9">E98*E98</f>
         <v>8883.4766893982887</v>
       </c>
       <c r="G98">

</xml_diff>